<commit_message>
updated tagged individuals from forest
</commit_message>
<xml_diff>
--- a/Exp_taggedHF.xlsx
+++ b/Exp_taggedHF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="338">
   <si>
     <t>ind</t>
   </si>
@@ -198,9 +198,6 @@
     <t>S_FAGGRA_H03</t>
   </si>
   <si>
-    <t>T_VIBCACE_H01</t>
-  </si>
-  <si>
     <t>T_VIBACE_H02</t>
   </si>
   <si>
@@ -697,6 +694,345 @@
   </si>
   <si>
     <t>T_FAGGRA_H13</t>
+  </si>
+  <si>
+    <t>S_FAGGRA_H05</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H09</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H10</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H11</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H14</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H15</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H12</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H16</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H12</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H13</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H13</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H05</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H07</t>
+  </si>
+  <si>
+    <t>1.7, 2.4</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H08</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H10</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H06</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H07</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H08</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H09</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H17</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H18</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H19</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H20</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H10</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H21</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H22</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H11</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H12</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H09</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H23</t>
+  </si>
+  <si>
+    <t>S_CORCOR_H24</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H08</t>
+  </si>
+  <si>
+    <t>T_FAGGRA_H14</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H13</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H10</t>
+  </si>
+  <si>
+    <t>1.0, 1.1</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H14</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H15</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H09</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H10</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H11</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H11</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H12</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H11</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H14</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H09</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H10</t>
+  </si>
+  <si>
+    <t>T_CORCOR_H16</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H11</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H12</t>
+  </si>
+  <si>
+    <t>T_FAGGRA_H15</t>
+  </si>
+  <si>
+    <t>T_FAGGRA_H16</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H11</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H12</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H13</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H13</t>
+  </si>
+  <si>
+    <t>S_FAGGRA_H06</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H15</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H16</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H14</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H15</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H16</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H17</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H18</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H19</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H20</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H17</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H18</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H12</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H19</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H20</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H13</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H14</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H15</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H09</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H21</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H10</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H21</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H16</t>
+  </si>
+  <si>
+    <t>S_ACEPEN_H12</t>
+  </si>
+  <si>
+    <t>T_ACEPEN_H16</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H22</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H13</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H22</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H14</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H14</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H11</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H23</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H14</t>
+  </si>
+  <si>
+    <t>S_VIBACE_H24</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H12</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H15</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H13</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H23</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H14</t>
+  </si>
+  <si>
+    <t>S_CAROVA_H24</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H15</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H16</t>
+  </si>
+  <si>
+    <t>T_ILEVER_H15</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H17</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H18</t>
+  </si>
+  <si>
+    <t>S_ILEVER_H16</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H15</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H16</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H19</t>
+  </si>
+  <si>
+    <t>T_CAROVA_H12</t>
+  </si>
+  <si>
+    <t>S_BETLEN_H20</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H17</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H18</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H19</t>
+  </si>
+  <si>
+    <t>S_HAMVIR_H20</t>
+  </si>
+  <si>
+    <t>T_VIBACE_H01</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D223"/>
+  <dimension ref="A1:D336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1212,7 +1548,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1240,7 +1576,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1307,7 +1643,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1425,7 +1761,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1456,22 +1792,22 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>5.4</v>
@@ -1479,7 +1815,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62">
         <v>3.5</v>
@@ -1487,12 +1823,12 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>1.8</v>
@@ -1500,7 +1836,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -1508,22 +1844,22 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1531,17 +1867,17 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>1.2</v>
@@ -1549,12 +1885,12 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>2.6</v>
@@ -1562,7 +1898,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>3.1</v>
@@ -1570,22 +1906,22 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>1.6</v>
@@ -1593,17 +1929,17 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>1.4</v>
@@ -1611,47 +1947,47 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>3.5</v>
@@ -1659,12 +1995,12 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>1.2</v>
@@ -1672,7 +2008,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>1.2</v>
@@ -1680,7 +2016,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>4.2</v>
@@ -1698,7 +2034,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B98">
         <v>2</v>
@@ -1706,7 +2042,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B99">
         <v>2.4</v>
@@ -1714,7 +2050,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>2.1</v>
@@ -1722,12 +2058,12 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B102">
         <v>2.1</v>
@@ -1735,7 +2071,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B103">
         <v>2.7</v>
@@ -1743,7 +2079,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B104">
         <v>2.5</v>
@@ -1751,12 +2087,12 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106">
         <v>1.3</v>
@@ -1764,45 +2100,45 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B114">
         <v>1.6</v>
@@ -1810,7 +2146,7 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>2.2999999999999998</v>
@@ -1818,27 +2154,27 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>4.5</v>
@@ -1846,7 +2182,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>2.1</v>
@@ -1854,27 +2190,27 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>1.3</v>
@@ -1882,7 +2218,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>2</v>
@@ -1890,7 +2226,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>6.9</v>
@@ -1898,12 +2234,12 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>2.5</v>
@@ -1911,7 +2247,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>2.7</v>
@@ -1919,15 +2255,15 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133">
         <v>2.1</v>
@@ -1935,7 +2271,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134">
         <v>2.4</v>
@@ -1943,22 +2279,22 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138">
         <v>3.5</v>
@@ -1966,62 +2302,62 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B150">
         <v>6.2</v>
@@ -2029,7 +2365,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B151">
         <v>5.6</v>
@@ -2037,17 +2373,17 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B154">
         <v>1.2</v>
@@ -2055,12 +2391,12 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B156">
         <v>7</v>
@@ -2068,32 +2404,32 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B162">
         <v>2.1</v>
@@ -2101,12 +2437,12 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B164">
         <v>2.4</v>
@@ -2114,22 +2450,22 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B168">
         <v>2.5</v>
@@ -2137,7 +2473,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B169">
         <v>2.1</v>
@@ -2145,7 +2481,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B170">
         <v>3.5</v>
@@ -2153,12 +2489,12 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B172">
         <v>2.7</v>
@@ -2166,7 +2502,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B173">
         <v>1.5</v>
@@ -2174,100 +2510,100 @@
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B192">
         <v>2</v>
@@ -2275,72 +2611,72 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B206">
         <v>2</v>
@@ -2348,12 +2684,12 @@
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B208">
         <v>1.2</v>
@@ -2361,22 +2697,22 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B212">
         <v>1.7</v>
@@ -2384,7 +2720,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B213">
         <v>1.9</v>
@@ -2392,47 +2728,47 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B222">
         <v>1.6</v>
@@ -2440,10 +2776,629 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B223">
         <v>1.8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>236</v>
+      </c>
+      <c r="B236">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>237</v>
+      </c>
+      <c r="B237" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>239</v>
+      </c>
+      <c r="B238">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>241</v>
+      </c>
+      <c r="B240">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>242</v>
+      </c>
+      <c r="B241">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>243</v>
+      </c>
+      <c r="B242">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>254</v>
+      </c>
+      <c r="B253">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>258</v>
+      </c>
+      <c r="B257">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>260</v>
+      </c>
+      <c r="B259" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>262</v>
+      </c>
+      <c r="B260">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>264</v>
+      </c>
+      <c r="B262">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>265</v>
+      </c>
+      <c r="B263">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>266</v>
+      </c>
+      <c r="B264">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>276</v>
+      </c>
+      <c r="B274">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>277</v>
+      </c>
+      <c r="B275">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>278</v>
+      </c>
+      <c r="B276">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>280</v>
+      </c>
+      <c r="B278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1">
+      <c r="A315" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1">
+      <c r="A317" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1">
+      <c r="A319" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>331</v>
+      </c>
+      <c r="B331">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>